<commit_message>
Se arregla el formato del documento y su contenido, se regenera el indice
</commit_message>
<xml_diff>
--- a/CSOF5303 Proyecto 3/Ciclo1/0926Diagramas.xlsx
+++ b/CSOF5303 Proyecto 3/Ciclo1/0926Diagramas.xlsx
@@ -8,9 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -7946,6 +7947,318 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Hoja1"/>
+      <sheetName val="Hoja2"/>
+      <sheetName val="Hoja3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="C1" t="str">
+            <v>Planeado</v>
+          </cell>
+          <cell r="D1" t="str">
+            <v>Real</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>Otros</v>
+          </cell>
+          <cell r="C2">
+            <v>0</v>
+          </cell>
+          <cell r="D2">
+            <v>16</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Inicio</v>
+          </cell>
+          <cell r="C3">
+            <v>1</v>
+          </cell>
+          <cell r="D3">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>Lanzamiento</v>
+          </cell>
+          <cell r="C4">
+            <v>27</v>
+          </cell>
+          <cell r="D4">
+            <v>29.5</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>Seguimiento</v>
+          </cell>
+          <cell r="C5">
+            <v>67.2</v>
+          </cell>
+          <cell r="D5">
+            <v>84</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>Estrategia</v>
+          </cell>
+          <cell r="C6">
+            <v>25</v>
+          </cell>
+          <cell r="D6">
+            <v>18</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>Plan</v>
+          </cell>
+          <cell r="C7">
+            <v>12.5</v>
+          </cell>
+          <cell r="D7">
+            <v>12.83</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>Requisitos</v>
+          </cell>
+          <cell r="C8">
+            <v>32</v>
+          </cell>
+          <cell r="D8">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>Diseño</v>
+          </cell>
+          <cell r="C9">
+            <v>20</v>
+          </cell>
+          <cell r="D9">
+            <v>8.33</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>Impl</v>
+          </cell>
+          <cell r="C10">
+            <v>117.5</v>
+          </cell>
+          <cell r="D10">
+            <v>72.83</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11" t="str">
+            <v>Pruebas</v>
+          </cell>
+          <cell r="C11">
+            <v>27</v>
+          </cell>
+          <cell r="D11">
+            <v>5.5</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12" t="str">
+            <v>Postmortem</v>
+          </cell>
+          <cell r="C12">
+            <v>15</v>
+          </cell>
+          <cell r="D12">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13" t="str">
+            <v>Doc</v>
+          </cell>
+          <cell r="C13">
+            <v>20</v>
+          </cell>
+          <cell r="D13">
+            <v>13</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="B34" t="str">
+            <v>Docu</v>
+          </cell>
+          <cell r="C34">
+            <v>172</v>
+          </cell>
+          <cell r="D34">
+            <v>61.27</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="B35" t="str">
+            <v>Impl</v>
+          </cell>
+          <cell r="C35">
+            <v>80</v>
+          </cell>
+          <cell r="D35">
+            <v>8.6199999999999992</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="B36" t="str">
+            <v>Legado</v>
+          </cell>
+          <cell r="C36">
+            <v>38</v>
+          </cell>
+          <cell r="D36">
+            <v>17.07</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="B37" t="str">
+            <v>OSB</v>
+          </cell>
+          <cell r="C37">
+            <v>62</v>
+          </cell>
+          <cell r="D37">
+            <v>32.51</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="B38" t="str">
+            <v>Planeación</v>
+          </cell>
+          <cell r="C38">
+            <v>94</v>
+          </cell>
+          <cell r="D38">
+            <v>115.8</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="B39" t="str">
+            <v>Presentación</v>
+          </cell>
+          <cell r="C39">
+            <v>22</v>
+          </cell>
+          <cell r="D39">
+            <v>30</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="B67" t="str">
+            <v>BPEL</v>
+          </cell>
+          <cell r="C67">
+            <v>50</v>
+          </cell>
+          <cell r="D67">
+            <v>47.8</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="B68" t="str">
+            <v>CRM</v>
+          </cell>
+          <cell r="C68">
+            <v>45</v>
+          </cell>
+          <cell r="D68">
+            <v>31.5</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="B69" t="str">
+            <v>Proceso</v>
+          </cell>
+          <cell r="C69">
+            <v>53</v>
+          </cell>
+          <cell r="D69">
+            <v>50.42</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="B70" t="str">
+            <v>Legado</v>
+          </cell>
+          <cell r="C70">
+            <v>22</v>
+          </cell>
+          <cell r="D70">
+            <v>11.35</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="B71" t="str">
+            <v>OSB</v>
+          </cell>
+          <cell r="C71">
+            <v>15</v>
+          </cell>
+          <cell r="D71">
+            <v>15.13</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="B72" t="str">
+            <v>Portal</v>
+          </cell>
+          <cell r="C72">
+            <v>10</v>
+          </cell>
+          <cell r="D72">
+            <v>15</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="B73" t="str">
+            <v>Producto</v>
+          </cell>
+          <cell r="C73">
+            <v>32</v>
+          </cell>
+          <cell r="D73">
+            <v>12</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="B74" t="str">
+            <v>Seguimiento</v>
+          </cell>
+          <cell r="C74">
+            <v>96</v>
+          </cell>
+          <cell r="D74">
+            <v>96</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8244,28 +8557,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>